<commit_message>
when same letter is guessed again, now not added to list twice, added option to tell a story during game loop, so child does not feel forced
</commit_message>
<xml_diff>
--- a/dictionaries/disclosures.xlsx
+++ b/dictionaries/disclosures.xlsx
@@ -19,11 +19,11 @@
   </sheets>
   <calcPr calcId="145621"/>
   <customWorkbookViews>
+    <customWorkbookView name="Rifca Peters - EWI - Personal View" guid="{0B508B25-7123-447E-9FD5-FE20BBAD71B2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="783" activeSheetId="1"/>
+    <customWorkbookView name="joost - Personal View" guid="{EDE4CE66-77B3-4DE9-B8E1-41F2D0C67E38}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
+    <customWorkbookView name="Franziska - Persoonlijke weergave" guid="{22AF5D13-DA6D-4567-8DD6-5735431A3EE3}" mergeInterval="0" personalView="1" maximized="1" xWindow="54" yWindow="-8" windowWidth="1320" windowHeight="784" activeSheetId="1"/>
+    <customWorkbookView name="Anika Boelhouwer - Personal View" guid="{D89975A1-9A50-491E-B44B-6A9DDF60C5E2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1676" windowHeight="825" activeSheetId="1" showComments="commIndAndComment"/>
     <customWorkbookView name="Franziska - Personal View" guid="{E9AA0514-4F1F-4D48-9ADD-4471FD4B0607}" mergeInterval="0" personalView="1" maximized="1" xWindow="54" yWindow="-8" windowWidth="1320" windowHeight="784" activeSheetId="2"/>
-    <customWorkbookView name="Anika Boelhouwer - Personal View" guid="{D89975A1-9A50-491E-B44B-6A9DDF60C5E2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1676" windowHeight="825" activeSheetId="1" showComments="commIndAndComment"/>
-    <customWorkbookView name="Franziska - Persoonlijke weergave" guid="{22AF5D13-DA6D-4567-8DD6-5735431A3EE3}" mergeInterval="0" personalView="1" maximized="1" xWindow="54" yWindow="-8" windowWidth="1320" windowHeight="784" activeSheetId="1"/>
-    <customWorkbookView name="joost - Personal View" guid="{EDE4CE66-77B3-4DE9-B8E1-41F2D0C67E38}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1936" windowHeight="1056" activeSheetId="1"/>
-    <customWorkbookView name="Rifca Peters - EWI - Personal View" guid="{0B508B25-7123-447E-9FD5-FE20BBAD71B2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1920" windowHeight="783" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1923,9 +1923,6 @@
     <t>grap</t>
   </si>
   <si>
-    <t>hockey</t>
-  </si>
-  <si>
     <t>doel</t>
   </si>
   <si>
@@ -1974,9 +1971,6 @@
     <t>vliegen</t>
   </si>
   <si>
-    <t>sportfilm</t>
-  </si>
-  <si>
     <t>klimrek</t>
   </si>
   <si>
@@ -2109,9 +2103,6 @@
     <t>ziekenhuis</t>
   </si>
   <si>
-    <t>boekenclub</t>
-  </si>
-  <si>
     <t>vandaag</t>
   </si>
   <si>
@@ -2169,9 +2160,6 @@
     <t>fontein</t>
   </si>
   <si>
-    <t>Ik hou van kinderen en leren hoe hun lichaam werkt, van het {name-hospital} en mijn school. Dit alles zorgt ervoor dat ik me heel belangrijk voel. Ik hou van mijn leven.</t>
-  </si>
-  <si>
     <t>trots</t>
   </si>
   <si>
@@ -2353,6 +2341,18 @@
   </si>
   <si>
     <t>energie</t>
+  </si>
+  <si>
+    <t>Ik hou van kinderen en leren hoe hun lichaam werkt, van het ziekenhuis en mijn school. Dit alles zorgt ervoor dat ik me heel belangrijk voel. Ik hou van mijn leven.</t>
+  </si>
+  <si>
+    <t>boek</t>
+  </si>
+  <si>
+    <t>bioscoop</t>
+  </si>
+  <si>
+    <t>stom</t>
   </si>
 </sst>
 </file>
@@ -2820,23 +2820,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{36463FEC-D002-4538-95B9-E15B5BF616EF}" diskRevisions="1" revisionId="507" version="17">
-  <header guid="{C4D08E0B-272C-419E-AAAE-5C9A2682FC84}" dateTime="2016-06-02T17:40:24" maxSheetId="5" userName="Rifca Peters - EWI" r:id="rId27" minRId="290" maxRId="340">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{3A84ED64-E2A8-43DB-97B4-A394FA63F920}" dateTime="2016-06-02T17:41:11" maxSheetId="5" userName="Rifca Peters - EWI" r:id="rId28">
-    <sheetIdMap count="4">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-      <sheetId val="3"/>
-      <sheetId val="4"/>
-    </sheetIdMap>
-  </header>
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{3B322AF9-1A2B-48FF-B7A6-D00B60D9D277}" diskRevisions="1" revisionId="520" version="22">
   <header guid="{9D2B0658-70B0-4FEA-AF87-74B776EB523B}" dateTime="2016-06-06T10:39:15" maxSheetId="5" userName="Franziska" r:id="rId29" minRId="341" maxRId="346">
     <sheetIdMap count="4">
       <sheetId val="1"/>
@@ -2949,12 +2933,147 @@
       <sheetId val="4"/>
     </sheetIdMap>
   </header>
+  <header guid="{2B84D422-1287-417A-BF1F-64052E494232}" dateTime="2016-07-03T21:12:57" maxSheetId="5" userName="Franziska" r:id="rId43" minRId="508" maxRId="515">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{3DB378D6-2A75-43F8-8833-AAACE116954C}" dateTime="2016-07-03T21:18:39" maxSheetId="5" userName="Franziska" r:id="rId44" minRId="516" maxRId="517">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{624A8B93-632D-44F6-B9DF-2D6B35866979}" dateTime="2016-07-03T22:02:42" maxSheetId="5" userName="Franziska" r:id="rId45" minRId="518">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{9EBAEEC1-8CE0-448F-A8A7-9061897659A2}" dateTime="2016-07-03T22:04:03" maxSheetId="5" userName="Franziska" r:id="rId46" minRId="519">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{3B322AF9-1A2B-48FF-B7A6-D00B60D9D277}" dateTime="2016-07-03T22:05:20" maxSheetId="5" userName="Franziska" r:id="rId47" minRId="520">
+    <sheetIdMap count="4">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+      <sheetId val="3"/>
+      <sheetId val="4"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
 <file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcmt sheetId="1" cell="G130" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Rifca Peters - EWI"/>
+  <rcc rId="508" sId="1">
+    <oc r="J26" t="inlineStr">
+      <is>
+        <t>P17</t>
+      </is>
+    </oc>
+    <nc r="J26" t="inlineStr">
+      <is>
+        <t>P4</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="509" sId="1">
+    <oc r="J38" t="inlineStr">
+      <is>
+        <t>P6</t>
+      </is>
+    </oc>
+    <nc r="J38" t="inlineStr">
+      <is>
+        <t>P4</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="510" sId="1">
+    <oc r="J39" t="inlineStr">
+      <is>
+        <t>P1</t>
+      </is>
+    </oc>
+    <nc r="J39" t="inlineStr">
+      <is>
+        <t>P14</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="511" sId="1">
+    <oc r="J59" t="inlineStr">
+      <is>
+        <t>P7</t>
+      </is>
+    </oc>
+    <nc r="J59" t="inlineStr">
+      <is>
+        <t>P11</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="512" sId="1">
+    <oc r="J60" t="inlineStr">
+      <is>
+        <t>P7</t>
+      </is>
+    </oc>
+    <nc r="J60" t="inlineStr">
+      <is>
+        <t>P8</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="513" sId="1">
+    <oc r="J66" t="inlineStr">
+      <is>
+        <t>P8</t>
+      </is>
+    </oc>
+    <nc r="J66" t="inlineStr">
+      <is>
+        <t>P7</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="514" sId="1">
+    <oc r="J63" t="inlineStr">
+      <is>
+        <t>P7</t>
+      </is>
+    </oc>
+    <nc r="J63" t="inlineStr">
+      <is>
+        <t>P9</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="515" sId="1">
+    <oc r="G68" t="inlineStr">
+      <is>
+        <t>Ik hou van kinderen en leren hoe hun lichaam werkt, van het {name-hospital} en mijn school. Dit alles zorgt ervoor dat ik me heel belangrijk voel. Ik hou van mijn leven.</t>
+      </is>
+    </oc>
+    <nc r="G68" t="inlineStr">
+      <is>
+        <t>Ik hou van kinderen en leren hoe hun lichaam werkt, van het ziekenhuis en mijn school. Dit alles zorgt ervoor dat ik me heel belangrijk voel. Ik hou van mijn leven.</t>
+      </is>
+    </nc>
+  </rcc>
 </revisions>
 </file>
 
@@ -4335,6 +4454,86 @@
       </border>
     </dxf>
   </rfmt>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog16.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="516" sId="1">
+    <oc r="J72" t="inlineStr">
+      <is>
+        <t>P7</t>
+      </is>
+    </oc>
+    <nc r="J72" t="inlineStr">
+      <is>
+        <t>P2</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="517" sId="1">
+    <oc r="J73" t="inlineStr">
+      <is>
+        <t>P4</t>
+      </is>
+    </oc>
+    <nc r="J73" t="inlineStr">
+      <is>
+        <t>P8</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog17.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="518" sId="1">
+    <oc r="M82" t="inlineStr">
+      <is>
+        <t>boekenclub</t>
+      </is>
+    </oc>
+    <nc r="M82" t="inlineStr">
+      <is>
+        <t>boek</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog18.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="519" sId="1">
+    <oc r="M121" t="inlineStr">
+      <is>
+        <t>sportfilm</t>
+      </is>
+    </oc>
+    <nc r="M121" t="inlineStr">
+      <is>
+        <t>bioscoop</t>
+      </is>
+    </nc>
+  </rcc>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog19.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="520" sId="1">
+    <oc r="M143" t="inlineStr">
+      <is>
+        <t>hockey</t>
+      </is>
+    </oc>
+    <nc r="M143" t="inlineStr">
+      <is>
+        <t>stom</t>
+      </is>
+    </nc>
+  </rcc>
 </revisions>
 </file>
 
@@ -4469,642 +4668,6 @@
       </is>
     </nc>
   </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog27.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="290" sId="1">
-    <oc r="G84" t="inlineStr">
-      <is>
-        <t>In het ziekenhuis wordt echt voor iedere robot gezorgd.</t>
-      </is>
-    </oc>
-    <nc r="G84" t="inlineStr">
-      <is>
-        <t>In het ziekenhuis wordt iedere robot goed verzorgd.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="291" sId="1">
-    <oc r="G81" t="inlineStr">
-      <is>
-        <t xml:space="preserve">In het ziekenhuis kun je er niet om heen om nieuwe mensen en robots te ontmoeten. Iedere dag komen nieuwe patienten binnen en af en toe ook nieuwe verpleegkundigen, artsen, of robots. </t>
-      </is>
-    </oc>
-    <nc r="G81" t="inlineStr">
-      <is>
-        <t xml:space="preserve">In het ziekenhuis ontmoet je vaak nieuwe mensen en robots. Iedere dag komen nieuwe patienten binnen en af en toe ook nieuwe verpleegkundigen of artsen. </t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="292" sId="1">
-    <oc r="G86" t="inlineStr">
-      <is>
-        <t>Ik hou van online games waarin je samen met andere spelers in een team speelt. Ik vind het leuker dan in mijn eentje strijden.</t>
-      </is>
-    </oc>
-    <nc r="G86" t="inlineStr">
-      <is>
-        <t>Ik hou van online games waarin je samen met andere spelers in een team speelt. Ik vind het leuker dan in mijn eentje spelen.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="293" sId="1">
-    <oc r="G93" t="inlineStr">
-      <is>
-        <t>Afgelopen week gingen we naar de dierentuin. Dat was echt fantastisch! I wou dat ik een aap was voor een dag.</t>
-      </is>
-    </oc>
-    <nc r="G93" t="inlineStr">
-      <is>
-        <t>Afgelopen week gingen we naar de dierentuin. Dat was echt fantastisch! Ik zou best graag voor een dag een aap willen zijn.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="294" sId="1">
-    <nc r="G94" t="inlineStr">
-      <is>
-        <t>Ik verheug me niet op mijn wekelijkse afspraak met de robotadviseur. Ze is aardig, maar ze heeft elkse week weer een lastige opdracht voor mij.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="295" sId="1">
-    <oc r="G96" t="inlineStr">
-      <is>
-        <t>Wil jij liever geen vrienden hebben of zoveel vrienden hebben dat je je hun namen niet meer kunt herinneren? Voor mij is het het laatste. Ik voel me erg snel eenzaam.</t>
-      </is>
-    </oc>
-    <nc r="G96" t="inlineStr">
-      <is>
-        <t>Zou jij liever geen vrienden hebben, of zoveel vrienden dat je hun namen niet meer kunt onthouden? Voor mij is het het laatste. Ik voel me erg snel eenzaam.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="296" sId="1">
-    <oc r="G100" t="inlineStr">
-      <is>
-        <t>Soms wou ik dat ik langer was, omdat ik dan mensen op ooghoogte zou kunnen ontmoeten en beter bij dingen zou kunnen.</t>
-      </is>
-    </oc>
-    <nc r="G100" t="inlineStr">
-      <is>
-        <t>Soms wou ik dat ik langer was, omdat ik dan mensen op ooghoogte kan ontmoeten en beter bij dingen kan.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="297" sId="1">
-    <oc r="G102" t="inlineStr">
-      <is>
-        <t>{name-friend} heeft een nieuwe gewoonte waarbij hij steeds films citeerd. Ik kijk niet veel naar films, dus weet ik nooit waar hij het over heeft. Het is zo stom.</t>
-      </is>
-    </oc>
-    <nc r="G102" t="inlineStr">
-      <is>
-        <t>{name-friend} heeft een nieuwe gewoonte, hij citeerd steeds uit films. Ik kijk niet veel naar films, dus weet ik nooit waar hij het over heeft. Het is zo stom.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="298" sId="1">
-    <oc r="G108" t="inlineStr">
-      <is>
-        <t>Er is een jongen die echt gewoon niet mijn vriend wil zijn. Ik weet niet wat ik verkeerd deed maar ik word er helemaal gek van. Waarom vindt hij me niet leuk?</t>
-      </is>
-    </oc>
-    <nc r="G108" t="inlineStr">
-      <is>
-        <t>Er is een jongen die echt niet mijn vriend wil zijn. Ik weet niet wat ik verkeerd doe maar ik word er helemaal gek van. Waarom vindt hij me niet leuk?</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="299" sId="1">
-    <oc r="G98" t="inlineStr">
-      <is>
-        <t>Ik geloof dat ik erg veel geluk heb. Ik heb gevonden wat ik tot het einde van mijn leven wil doen en ik denk dat ik er zelfs goed in ben.</t>
-      </is>
-    </oc>
-    <nc r="G98" t="inlineStr">
-      <is>
-        <t>Ik geloof dat ik erg veel geluk heb. Wat ik doe wil ik tot het einde van mijn leven doen en ik denk dat ik er ook goed in ben.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="300" sId="1">
-    <oc r="G99" t="inlineStr">
-      <is>
-        <t>Ik hou van mijn baan. Vooral praten met kinderen zoals jou is leuk. Ik leer graag meer over jou en jouw leven.</t>
-      </is>
-    </oc>
-    <nc r="G99" t="inlineStr">
-      <is>
-        <t>Ik hou van mijn werk Vooral praten met kinderen zoals jou is leuk. Ik leer graag meer over jou en jouw leven.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="301" sId="1">
-    <oc r="G105" t="inlineStr">
-      <is>
-        <t>Eerst was ik heel boos op {name-owner} aangezien hij me op zolder plaatste. Maar nu heb ik hem vergeven. Ik denk dat het niet de bedoeling was me te kwetsen.</t>
-      </is>
-    </oc>
-    <nc r="G105" t="inlineStr">
-      <is>
-        <t>Eerst was ik heel boos op {name-owner} aangezien hij me op zolder plaatste. Maar nu heb ik hem vergeven. Ik denk dat het niet zijn bedoeling was me te kwetsen.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="302" sId="1">
-    <oc r="G107" t="inlineStr">
-      <is>
-        <t>Ik kan niet goed met kritiek omgaan. Het maakt me van steek. Soms word ik boos, dan neem ik wraak, en soms word ik verdrietig, dan huil ik. Ik moet leren er  beter mee om te gaan.</t>
-      </is>
-    </oc>
-    <nc r="G107" t="inlineStr">
-      <is>
-        <t>Ik kan niet goed met kritiek omgaan. Het maakt me van steek. Soms word ik boos, dan neem ik wraak, en soms word ik verdrietig, dan huil ik. Ik moet hier beter mee leren omgaan.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="303" sId="1">
-    <oc r="G110" t="inlineStr">
-      <is>
-        <t>Wanneer ik hard aan het werken ben of erg zenuwachtig ben, oververhit ik en soms wordt ik zelfs bewusteloos. Het is zo beschamend!</t>
-      </is>
-    </oc>
-    <nc r="G110" t="inlineStr">
-      <is>
-        <t>Wanneer ik hard aan het werken ben of erg zenuwachtig ben, oververhit ik en wordt ik soms zelfs bewusteloos. Ik schaam me hier erg voor!</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="304" sId="1">
-    <oc r="G112" t="inlineStr">
-      <is>
-        <t>Ik maak altijd grappen over {name-friend}'s grote hoofd. Ik denk dat dit de reden is waarom hij nu steeds een muts draagt. Ik weet dat ik me zou moeten verontschuldigen maar ik vind dat hij er beter mee uitziet.</t>
-      </is>
-    </oc>
-    <nc r="G112" t="inlineStr">
-      <is>
-        <t>Ik maak altijd grappen over {name-friend}'s grote hoofd. Ik denk dat dit de reden is waarom hij nu steeds een muts draagt. Ik weet dat ik me zou moeten verontschuldigen maar ik vind dat hij er beter uitziet met muts.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="305" sId="1">
-    <oc r="G113" t="inlineStr">
-      <is>
-        <t xml:space="preserve"> {name-owner} nam me een keer mee naar een robotgevecht. Iemand zei tegen mij dat hij {name-owner} pijn zou doen als ik won. Ik won en ze zijn {name-owner} aangevallen. Ik probeer er niet meer aan te denken.</t>
-      </is>
-    </oc>
-    <nc r="G113" t="inlineStr">
-      <is>
-        <t xml:space="preserve"> {name-owner} nam me een keer mee naar een robotgevecht. Iemand zei tegen mij dat hij {name-owner} pijn zou doen als ik won. Ik won en ze hebben {name-owner} aangevallen. Ik probeer er niet meer aan te denken.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="306" sId="1">
-    <oc r="G104" t="inlineStr">
-      <is>
-        <t xml:space="preserve">Ik hou echt van deze ene verpleegkundige, zuster {name-nurse}. Zij is anders dan alle mensen die ik ken. Wanneer ze in de buurt is,moet ik ervoor  zorgen dat ze me opmerkt. </t>
-      </is>
-    </oc>
-    <nc r="G104" t="inlineStr">
-      <is>
-        <t xml:space="preserve">Ik hou echt van verpleegkundige {name-nurse}. Zij is anders dan alle andere mensen die ik ken. Wanneer ze in de buurt is, zorg ik ervoor dat ze me opmerkt. </t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="307" sId="1">
-    <oc r="G114" t="inlineStr">
-      <is>
-        <t>Ik zag een keer een aantal mensen een sport doen die ik nog nooit tevoren heb gezien. Ze vertelden mij dat het Bowlen heet.</t>
-      </is>
-    </oc>
-    <nc r="G114" t="inlineStr">
-      <is>
-        <t>Ik zag een keer een aantal mensen een sport doen die ik nog nooit eerder heb gezien. Ze vertelden mij dat het Bowlen heet.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="308" sId="1">
-    <oc r="G115" t="inlineStr">
-      <is>
-        <t>{name-owner} nam me soms mee naar voetbaltrainingen. Ik kan niet met mensen spelen. Ze zijn te groot en te snel. Dus ik kon alleen toekijken.</t>
-      </is>
-    </oc>
-    <nc r="G115" t="inlineStr">
-      <is>
-        <t>{name-owner} nam me soms mee naar de training van voetbal. Ik kan niet met mensen voetballen. Ze zijn te groot en te snel. Dus kon ik alleen toekijken.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="309" sId="1">
-    <oc r="G119" t="inlineStr">
-      <is>
-        <t>Robots zijn erg onhandig. Dus kunnen we maar een beperkt aantal sporten doen.</t>
-      </is>
-    </oc>
-    <nc r="G119" t="inlineStr">
-      <is>
-        <t>Robots zijn some wat onhandig. Dus kunnen we maar een beperkt aantal sporten doen.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="310" sId="1">
-    <oc r="G124" t="inlineStr">
-      <is>
-        <t>Ik denk echt dat geld een te grote invloed heeft op professionele robotsporten. Soms verliezen robots met opzet vanwege geld.</t>
-      </is>
-    </oc>
-    <nc r="G124" t="inlineStr">
-      <is>
-        <t>Ik denk echt dat geld een te veel invloed heeft op professionele robotsporten. Soms verliezen robots expres vanwege geld.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="311" sId="1">
-    <oc r="G125" t="inlineStr">
-      <is>
-        <t>Ik hou niet van sporten die men slechts voor het uithoudingsvermogen doet. Ze lijken gewoon erg saai. Je bent alleen en doet de hele tijd hetzelfde.</t>
-      </is>
-    </oc>
-    <nc r="G125" t="inlineStr">
-      <is>
-        <t>Ik hou niet van conditie sporten. Ze lijken mij erg saai. Je bent alleen en doet de hele tijd hetzelfde.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="312" sId="1">
-    <oc r="G129" t="inlineStr">
-      <is>
-        <t>Ik hou niet van erg competitieve sporten of spelers. Bij het sporten zou het plezier belangrijker moeten zijn dan het winnen.</t>
-      </is>
-    </oc>
-    <nc r="G129" t="inlineStr">
-      <is>
-        <t>Ik hou niet van erg competitieve sporten of spelers. Bij het sporten is plezier belangrijker dan winnen.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="1" sqref="G130" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcmt sheetId="1" cell="G124" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Rifca Peters - EWI"/>
-  <rcc rId="313" sId="1">
-    <oc r="G120" t="inlineStr">
-      <is>
-        <t>Soms ga ik graag wat op het klimrek spelen na school en voor ik met mijn huiswerk begin. Het zorgt ervoor dat ik beter kan denken.</t>
-      </is>
-    </oc>
-    <nc r="G120" t="inlineStr">
-      <is>
-        <t>Soms ga ik na school op het klimrek spelen voor ik met mijn huiswerk begin. Het zorgt ervoor dat ik beter kan denken.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="314" sId="1">
-    <oc r="G127" t="inlineStr">
-      <is>
-        <t>Als ik een sport voor een dag zou kunnen proberen, wetend dat het niet zou kunnen mislukken, zou ik voor base jumpen kiezen. Dat is dicht bij echt vliegen.</t>
-      </is>
-    </oc>
-    <nc r="G127" t="inlineStr">
-      <is>
-        <t>Als ik een sport voor een dag zou kunnen proberen, en het kan niet mislukken, dan zou ik voor base jumpen kiezen. Dat is dicht bij echt vliegen.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="315" sId="1">
-    <oc r="G128" t="inlineStr">
-      <is>
-        <t>Ik vind het heel belangrijk dat robots fit blijven. We hebben lichamen om ze te gebruiken.</t>
-      </is>
-    </oc>
-    <nc r="G128" t="inlineStr">
-      <is>
-        <t>Ik vind het heel belangrijk dat robots fit blijven. We hebben een lichaam om te gebruiken.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="316" sId="1">
-    <oc r="G123" t="inlineStr">
-      <is>
-        <t>Veel robots raken gemakkelijk beschadigd maar ik probeer erg voorzichtig te zijn. Om deze reden doe ik niet aan ruige sporten.</t>
-      </is>
-    </oc>
-    <nc r="G123" t="inlineStr">
-      <is>
-        <t>Veel robots gaan snel stuk maar ik probeer erg voorzichtig te zijn. Om deze reden doe ik niet aan ruige sporten.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="317" sId="1">
-    <oc r="G136" t="inlineStr">
-      <is>
-        <t>Het ergert me erg dat iedereen van mijn klasgenoten en mijn robotvrienden een voetbalobsessie hebben. Zij geven niet eens een andere sport de kans.</t>
-      </is>
-    </oc>
-    <nc r="G136" t="inlineStr">
-      <is>
-        <t>Ik vind het vervelend dat al mijn klasgenoten en robotvrienden een voetbalobsessie hebben. Zij geven niet eens een andere sport de kans.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="318" sId="1">
-    <oc r="G137" t="inlineStr">
-      <is>
-        <t>Het maakt me verdrietig dat NAOs niet waterdicht zijn. Ik zou het leuk vinden om zwemmen , duiken of surfen ook eens te kunnen proberen.</t>
-      </is>
-    </oc>
-    <nc r="G137" t="inlineStr">
-      <is>
-        <t>Het maakt me verdrietig dat NAOs niet waterdicht zijn. Ik zou het leuk vinden om zwemmen , duiken of surfen te kunnen proberen.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="319" sId="1">
-    <oc r="G130" t="inlineStr">
-      <is>
-        <t>In mijn Basketbalteam ben ik de power-forward. Ik vind het leuk, maar het betekend ook dat ik vaak zou moeten scoren. Dat doe ik niet.</t>
-      </is>
-    </oc>
-    <nc r="G130" t="inlineStr">
-      <is>
-        <t xml:space="preserve">In mijn Basketbalteam ben ik de power-forward. Ik vind het leuk, maar het betekend ook dat ik vaak zou moeten scoren. Dat doe ik niet. </t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="320" sId="1">
-    <oc r="G126" t="inlineStr">
-      <is>
-        <t>Ik hield van onze laatste basketbaltrainer. Ik vertelde haar over mijn oververhittingsprobleem en hoe erg ik er last van had, en zij nam de tijd om het iedere teamgenoot persoonlijk uit te leggen. Ik mis haar erg.</t>
-      </is>
-    </oc>
-    <nc r="G126" t="inlineStr">
-      <is>
-        <t>Ik hield van onze vorige basketbaltrainer. Ik vertelde haar over mijn oververhittingsprobleem en hoe erg ik er last van had, en zij nam de tijd om het aan alle teamgenoten persoonlijk uit te leggen. Ik mis haar erg.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="321" sId="1">
-    <oc r="G132" t="inlineStr">
-      <is>
-        <t>Bij onze laatste Karate-training heb ik tegen de leraar gewonnen. Dat was helemaal fantastisch en onverwacht. Ik geloof dat ik me de laatste tijd echt heb verbeterd.</t>
-      </is>
-    </oc>
-    <nc r="G132" t="inlineStr">
-      <is>
-        <t>Bij onze laatste Karate-training heb ik van de leraar gewonnen. Dat was helemaal fantastisch en onverwacht. Ik geloof dat ik me de laatste tijd echt beter ben geworden.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="322" sId="1">
-    <oc r="G134" t="inlineStr">
-      <is>
-        <t xml:space="preserve">Toen ik s'morgens een keer  gymnastiekoefeningen deed, is iets raars gebeurt. Plotseling voelde ik me helemaal licht. Ik had geen enkele zorgen meer. Ik probeer het iedere keer opnieuw te ervaren, maar helaas. </t>
-      </is>
-    </oc>
-    <nc r="G134" t="inlineStr">
-      <is>
-        <t xml:space="preserve">Op een morgen, toen ik gymnastiekoefeningen deed, is er iets raars gebeurt. Plotseling voelde ik me helemaal licht. Ik had geen enkele zorgen meer. Ik probeer het iedere keer opnieuw te ervaren, maar helaas. </t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="323" sId="1">
-    <oc r="G138" t="inlineStr">
-      <is>
-        <t>Hoe erg ik ook voetbal haat, het is uiteindelijk een nuttig onderwerp om  met sommige mensen en robots een gesprek te beginnen. Dus ik ben stiekem wel blij dat mijn vrienden me dwingen op de hoogte te blijven.</t>
-      </is>
-    </oc>
-    <nc r="G138" t="inlineStr">
-      <is>
-        <t>Hoe erg ik voetbal ook haat, het is uiteindelijk een nuttig onderwerp om  met sommige mensen en robots een gesprek te beginnen. Dus ik ben stiekem wel blij dat mijn vrienden me dwingen op de hoogte te blijven.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="324" sId="1">
-    <oc r="G142" t="inlineStr">
-      <is>
-        <t>Ik haat {name-friend}! Hij weet dat ik niet van voetbal hou. Vandaag speelde ik alleen voor hem, maar toen ik het doel miste lachte hij me uit en noemde me een sukkel.</t>
-      </is>
-    </oc>
-    <nc r="G142" t="inlineStr">
-      <is>
-        <t>Ik haat {name-friend}! Hij weet dat ik niet van voetbal hou. Vandaag ging ik voor hem toch mee voetballen, maar toen ik het doel miste lachte hij me uit en noemde me een sukkel.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="325" sId="1">
-    <oc r="G143" t="inlineStr">
-      <is>
-        <t>Gisteren ben ik met basketbal gestopt en heb ik mijn team teleurgesteld. Ik vertelde hun dat het komt omdat we nooit winnen. Dat was het stomste wat ik had kunnen zeggen. Ik haat mezelf.</t>
-      </is>
-    </oc>
-    <nc r="G143" t="inlineStr">
-      <is>
-        <t>Gisteren ben ik met basketbal gestopt en heb ik mijn team teleurgesteld. Ik vertelde hun dat ik ben gestopt omdat we nooit winnen. Dat was het stomste wat ik had kunnen zeggen. Ik haat mezelf.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="326" sId="1">
-    <oc r="G146" t="inlineStr">
-      <is>
-        <t xml:space="preserve">Ik hou van dansen! Maar niemand mag er achterkomen! Mijn vrienden lachen dansende robots steeds maar uit. </t>
-      </is>
-    </oc>
-    <nc r="G146" t="inlineStr">
-      <is>
-        <t xml:space="preserve">Ik hou van dansen! Maar niemand mag er achterkomen! Mijn vrienden lachen dansende robots steeds uit. </t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="327" sId="1">
-    <oc r="G148" t="inlineStr">
-      <is>
-        <t xml:space="preserve">Mijn basketbaltrainer maakte vaak grappen over mijn hitteprobleem en mijn onhandigheid. Soms zouden mijn teamgenoten me duwen, alleen omdat hij dan in de lach schiet. </t>
-      </is>
-    </oc>
-    <nc r="G148" t="inlineStr">
-      <is>
-        <t xml:space="preserve">Mijn basketbaltrainer maakte vaak grappen over mijn hitteprobleem en mijn onhandigheid. Soms duwen mijn teamgenoten mij, alleen omdat hij dan in de lach schiet. </t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="328" sId="1">
-    <oc r="G46" t="inlineStr">
-      <is>
-        <t>Robots kunne goed leren omdat wij makkelijk dingen onthouden. Lessen gaan dus vaker over dingen doen dan over dingen onthouden.</t>
-      </is>
-    </oc>
-    <nc r="G46" t="inlineStr">
-      <is>
-        <t>Robots kunnen goed leren omdat wij makkelijk dingen onthouden. Lessen gaan dus vaker over dingen doen dan over dingen onthouden.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="329" sId="1">
-    <oc r="G67" t="inlineStr">
-      <is>
-        <t>Ik denk dat Dr. {name-dr} teleurgesteld is in mij. Ik doe mijn best, maar ik maak nog te vaak fouten. Mensen zijn niet altijd makkelijk om te begrijpen.</t>
-      </is>
-    </oc>
-    <nc r="G67" t="inlineStr">
-      <is>
-        <t>Ik denk dat dokter {name-dr} teleurgesteld is in mij. Ik doe mijn best, maar ik maak nog te vaak fouten. Mensen zijn niet altijd makkelijk om te begrijpen.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="330" sId="1">
-    <oc r="G8" t="inlineStr">
-      <is>
-        <t>Dr. {name-dr} is mijn mentor. {dr-gender-pn} leert me alles over diabetes en kinderen en {dr-gender-pn} weet veel!</t>
-      </is>
-    </oc>
-    <nc r="G8" t="inlineStr">
-      <is>
-        <t>Dokter {name-dr} is mijn mentor. {dr-gender-pn} leert me alles over diabetes en kinderen en {dr-gender-pn} weet veel!</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="331" sId="1">
-    <oc r="G64" t="inlineStr">
-      <is>
-        <t>Afgelopen jaar was ik de beste robot in drie vakken op school. Ik wil niet opscheppen, maar het voelde echt goed. Dr. {name-dr} was heel trots op mij.</t>
-      </is>
-    </oc>
-    <nc r="G64" t="inlineStr">
-      <is>
-        <t>Afgelopen jaar was ik de beste robot in drie vakken op school. Ik wil niet opscheppen, maar het voelde echt goed. Dokter {name-dr} was heel trots op mij.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="332" sId="1">
-    <oc r="G69" t="inlineStr">
-      <is>
-        <t>Zuster {name-nurse} heeft al eens mijn leven gered toen {name-r3} in de pauze probeerde me in de fontein te duwen. Dat zal ik nooit vergeten.</t>
-      </is>
-    </oc>
-    <nc r="G69" t="inlineStr">
-      <is>
-        <t>Verpleegkundige {name-nurse} heeft al eens mijn leven gered toen {name-r3} in de pauze probeerde me in de fontein te duwen. Dat zal ik nooit vergeten.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcmt sheetId="1" cell="G69" guid="{00000000-0000-0000-0000-000000000000}" action="delete" author="Rifca Peters - EWI"/>
-  <rcc rId="333" sId="1">
-    <oc r="G76" t="inlineStr">
-      <is>
-        <t>Ik moest een keer met een andere robot samenwerken en hij deed er helemaal niks aan. Toen heb ik zijn naam niet op het papier gezet, terwijl ik tegen hem zei dat ik het wel zou doen.</t>
-      </is>
-    </oc>
-    <nc r="G76" t="inlineStr">
-      <is>
-        <t>Ik moest een keer met een andere robot samenwerken en hij deed helemaal niks. Toen heb ik zijn naam niet op het papier gezet, terwijl ik tegen hem zei dat ik het wel zou doen.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="334" sId="1">
-    <oc r="G90" t="inlineStr">
-      <is>
-        <t>Iets dat me echt ergert is het geluid van slippers. Gelukkiger dragen mensen ze alleen maar tijdens het zomer.</t>
-      </is>
-    </oc>
-    <nc r="G90" t="inlineStr">
-      <is>
-        <t>Ik erger mij aan het geluid van slippers. Gelukkiger dragen mensen ze alleen maar tijdens de zomer.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="335" sId="1">
-    <oc r="G92" t="inlineStr">
-      <is>
-        <t>Ik denk dat ik doctor {name-dr} vraag of {name-r2} tijdens het volgende semester naar onze kamer kan verhuizen. Ze lijkt me erg aardig en {name-sis} en {name-friend} vinden haar ook leuk.</t>
-      </is>
-    </oc>
-    <nc r="G92" t="inlineStr">
-      <is>
-        <t>Ik denk dat ik dokter {name-dr} vraag of {name-r2} tijdens het volgende semester naar onze kamer kan verhuizen. Ze lijkt me erg aardig en {name-sis} en {name-friend} vinden haar ook leuk.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="336" sId="1">
-    <oc r="G94" t="inlineStr">
-      <is>
-        <t>Ik verheug me niet echt op mijn wekelijkse afspraak met de robotadviseur. Ze is aardig, maar ze stelt iedere keer een wekelijkse uitdaging voor mij.</t>
-      </is>
-    </oc>
-    <nc r="G94" t="inlineStr">
-      <is>
-        <t>Ik verheug me niet op mijn wekelijkse afspraak met de robotadviseur. Ze is aardig, maar ze heeft elke week weer een uitdagende opdracht voor mij.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="1" sqref="G73" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="1" sqref="F73" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="337" sId="1">
-    <oc r="G74" t="inlineStr">
-      <is>
-        <t>Ik ben een keer tijdens een schoolreis bewusteloos geraakt. Niemand wist wat ze met me moesten  doen, dus hebben ze me terug naar het ziekenhuis gebracht. Ik heb de reis voor iedereen verpest.</t>
-      </is>
-    </oc>
-    <nc r="G74" t="inlineStr">
-      <is>
-        <t>Ik ben een keer tijdens een schoolreisje bewusteloos geraakt. Niemand wist wat ze met me moesten  doen, dus hebben ze me terug naar het ziekenhuis gebracht. Ik heb de reis voor iedereen verpest.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="338" sId="1">
-    <oc r="G82" t="inlineStr">
-      <is>
-        <t>Gisteren werd ik door drie van mijn klasgenoten gevraagd of ik bij hun boekenclub wilde horen. Maargoed, ze vroegen iedereen.</t>
-      </is>
-    </oc>
-    <nc r="G82" t="inlineStr">
-      <is>
-        <t>Gisteren vroegen drie van mijn klasgenoten of ik bij hun boekenclub wilde horen. Maargoed, ze vroegen iedereen.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="339" sId="1">
-    <oc r="G149" t="inlineStr">
-      <is>
-        <t>Helaas kan ik op dit moment niets spannends verzinnen dat ik jou zou kunnen vertellen.</t>
-      </is>
-    </oc>
-    <nc r="G149" t="inlineStr">
-      <is>
-        <t>Op dit moment weet ik helaas niets spannends om jou te vertellen.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="340" sId="1">
-    <oc r="G89" t="inlineStr">
-      <is>
-        <t>Ik vind het leuk als kinderen met hun ouders bevriend kunnen zijn. Maar het schijnt niet altijd mogelijk te zijn.</t>
-      </is>
-    </oc>
-    <nc r="G89" t="inlineStr">
-      <is>
-        <t>Ik vind het leuk als kinderen en hun ouders vrienden zijn. Maar het schijnt niet altijd mogelijk te zijn.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcv guid="{0B508B25-7123-447E-9FD5-FE20BBAD71B2}" action="add"/>
 </revisions>
 </file>
 
@@ -6029,21 +5592,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A141" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M144" sqref="M144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" customWidth="1"/>
-    <col min="6" max="6" width="38" customWidth="1"/>
+    <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="38" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="38" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="8" customWidth="1"/>
     <col min="10" max="10" width="20.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="20.85546875" customWidth="1"/>
     <col min="13" max="13" width="15.85546875" customWidth="1"/>
@@ -6122,7 +5686,7 @@
         <v>379</v>
       </c>
       <c r="M2" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -6157,7 +5721,7 @@
         <v>379</v>
       </c>
       <c r="M3" s="127" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -6192,7 +5756,7 @@
         <v>379</v>
       </c>
       <c r="M4" s="127" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -6227,7 +5791,7 @@
         <v>379</v>
       </c>
       <c r="M5" s="127" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -6262,7 +5826,7 @@
         <v>379</v>
       </c>
       <c r="M6" s="127" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -6297,7 +5861,7 @@
         <v>379</v>
       </c>
       <c r="M7" s="127" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -6332,7 +5896,7 @@
         <v>379</v>
       </c>
       <c r="M8" s="127" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6367,7 +5931,7 @@
         <v>379</v>
       </c>
       <c r="M9" s="127" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6402,7 +5966,7 @@
         <v>379</v>
       </c>
       <c r="M10" s="127" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -6437,7 +6001,7 @@
         <v>379</v>
       </c>
       <c r="M11" s="127" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -6472,7 +6036,7 @@
         <v>379</v>
       </c>
       <c r="M12" s="127" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -6507,7 +6071,7 @@
         <v>379</v>
       </c>
       <c r="M13" s="127" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -6533,7 +6097,7 @@
         <v>414</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
       <c r="K14" s="127" t="s">
         <v>340</v>
@@ -6542,7 +6106,7 @@
         <v>379</v>
       </c>
       <c r="M14" s="127" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -6577,7 +6141,7 @@
         <v>379</v>
       </c>
       <c r="M15" s="127" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -6612,7 +6176,7 @@
         <v>379</v>
       </c>
       <c r="M16" s="127" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -6647,7 +6211,7 @@
         <v>379</v>
       </c>
       <c r="M17" s="127" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -6685,7 +6249,7 @@
         <v>379</v>
       </c>
       <c r="M18" s="127" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -6720,7 +6284,7 @@
         <v>379</v>
       </c>
       <c r="M19" s="127" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -6755,7 +6319,7 @@
         <v>379</v>
       </c>
       <c r="M20" s="127" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -6790,7 +6354,7 @@
         <v>379</v>
       </c>
       <c r="M21" s="127" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -6825,7 +6389,7 @@
         <v>379</v>
       </c>
       <c r="M22" s="127" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
     </row>
     <row r="23" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -6860,7 +6424,7 @@
         <v>379</v>
       </c>
       <c r="M23" s="127" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
     </row>
     <row r="24" spans="1:13" s="128" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -6895,7 +6459,7 @@
         <v>379</v>
       </c>
       <c r="M24" s="128" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -6930,7 +6494,7 @@
         <v>379</v>
       </c>
       <c r="M25" s="127" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -6965,7 +6529,7 @@
         <v>379</v>
       </c>
       <c r="M26" s="127" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
     </row>
     <row r="27" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -7000,7 +6564,7 @@
         <v>379</v>
       </c>
       <c r="M27" s="127" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
     </row>
     <row r="28" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -7035,7 +6599,7 @@
         <v>379</v>
       </c>
       <c r="M28" s="127" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
     </row>
     <row r="29" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -7070,7 +6634,7 @@
         <v>379</v>
       </c>
       <c r="M29" s="127" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
     </row>
     <row r="30" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -7105,7 +6669,7 @@
         <v>379</v>
       </c>
       <c r="M30" s="127" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
     </row>
     <row r="31" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -7140,7 +6704,7 @@
         <v>379</v>
       </c>
       <c r="M31" s="127" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
     </row>
     <row r="32" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -7166,7 +6730,7 @@
         <v>411</v>
       </c>
       <c r="J32" s="19" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="K32" s="127" t="s">
         <v>340</v>
@@ -7175,7 +6739,7 @@
         <v>379</v>
       </c>
       <c r="M32" s="127" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
     </row>
     <row r="33" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -7201,7 +6765,7 @@
         <v>399</v>
       </c>
       <c r="J33" s="20" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="K33" s="127" t="s">
         <v>340</v>
@@ -7210,7 +6774,7 @@
         <v>379</v>
       </c>
       <c r="M33" s="127" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
     </row>
     <row r="34" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -7245,7 +6809,7 @@
         <v>379</v>
       </c>
       <c r="M34" s="127" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -7280,7 +6844,7 @@
         <v>379</v>
       </c>
       <c r="M35" s="127" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
     </row>
     <row r="36" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -7315,7 +6879,7 @@
         <v>379</v>
       </c>
       <c r="M36" s="127" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -7350,7 +6914,7 @@
         <v>379</v>
       </c>
       <c r="M37" s="127" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -7385,7 +6949,7 @@
         <v>379</v>
       </c>
       <c r="M38" s="127" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
     </row>
     <row r="39" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -7420,7 +6984,7 @@
         <v>379</v>
       </c>
       <c r="M39" s="127" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
     </row>
     <row r="40" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -7455,7 +7019,7 @@
         <v>379</v>
       </c>
       <c r="M40" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
     </row>
     <row r="41" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -7493,7 +7057,7 @@
         <v>379</v>
       </c>
       <c r="M41" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -7528,7 +7092,7 @@
         <v>379</v>
       </c>
       <c r="M42" s="127" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
     </row>
     <row r="43" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -7563,7 +7127,7 @@
         <v>379</v>
       </c>
       <c r="M43" s="127" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
     </row>
     <row r="44" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -7598,7 +7162,7 @@
         <v>379</v>
       </c>
       <c r="M44" s="127" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
     </row>
     <row r="45" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -7633,7 +7197,7 @@
         <v>379</v>
       </c>
       <c r="M45" s="127" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
     </row>
     <row r="46" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -7668,7 +7232,7 @@
         <v>379</v>
       </c>
       <c r="M46" s="127" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
     </row>
     <row r="47" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -7703,7 +7267,7 @@
         <v>379</v>
       </c>
       <c r="M47" s="127" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
     </row>
     <row r="48" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -7738,7 +7302,7 @@
         <v>379</v>
       </c>
       <c r="M48" s="127" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -7773,7 +7337,7 @@
         <v>379</v>
       </c>
       <c r="M49" s="127" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -7808,7 +7372,7 @@
         <v>379</v>
       </c>
       <c r="M50" s="127" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -7843,7 +7407,7 @@
         <v>379</v>
       </c>
       <c r="M51" s="127" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -7878,7 +7442,7 @@
         <v>379</v>
       </c>
       <c r="M52" s="127" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -7904,7 +7468,7 @@
         <v>419</v>
       </c>
       <c r="J53" s="37" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="K53" s="127" t="s">
         <v>340</v>
@@ -7913,7 +7477,7 @@
         <v>379</v>
       </c>
       <c r="M53" s="127" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -7939,7 +7503,7 @@
         <v>414</v>
       </c>
       <c r="J54" s="39" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="K54" s="127" t="s">
         <v>340</v>
@@ -7948,7 +7512,7 @@
         <v>379</v>
       </c>
       <c r="M54" s="127" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
     </row>
     <row r="55" spans="1:13" s="128" customFormat="1" ht="90" x14ac:dyDescent="0.25">
@@ -7983,7 +7547,7 @@
         <v>379</v>
       </c>
       <c r="M55" s="128" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
     </row>
     <row r="56" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -8018,7 +7582,7 @@
         <v>379</v>
       </c>
       <c r="M56" s="127" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -8053,7 +7617,7 @@
         <v>379</v>
       </c>
       <c r="M57" s="127" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -8091,7 +7655,7 @@
         <v>379</v>
       </c>
       <c r="M58" s="127" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -8117,7 +7681,7 @@
         <v>413</v>
       </c>
       <c r="J59" s="43" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K59" s="127" t="s">
         <v>340</v>
@@ -8126,7 +7690,7 @@
         <v>379</v>
       </c>
       <c r="M59" s="127" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -8164,7 +7728,7 @@
         <v>379</v>
       </c>
       <c r="M60" s="127" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8199,7 +7763,7 @@
         <v>379</v>
       </c>
       <c r="M61" s="127" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -8225,7 +7789,7 @@
         <v>434</v>
       </c>
       <c r="J62" s="46" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="K62" s="127" t="s">
         <v>340</v>
@@ -8234,7 +7798,7 @@
         <v>379</v>
       </c>
       <c r="M62" s="127" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
     </row>
     <row r="63" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -8272,7 +7836,7 @@
         <v>379</v>
       </c>
       <c r="M63" s="127" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
     </row>
     <row r="64" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -8295,7 +7859,7 @@
         <v>125</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>711</v>
+        <v>769</v>
       </c>
       <c r="I64" t="s">
         <v>409</v>
@@ -8310,7 +7874,7 @@
         <v>379</v>
       </c>
       <c r="M64" s="127" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="65" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -8348,7 +7912,7 @@
         <v>379</v>
       </c>
       <c r="M65" s="127" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
     </row>
     <row r="66" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -8383,7 +7947,7 @@
         <v>379</v>
       </c>
       <c r="M66" s="127" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
     </row>
     <row r="67" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -8418,7 +7982,7 @@
         <v>379</v>
       </c>
       <c r="M67" s="127" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
     </row>
     <row r="68" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8444,7 +8008,7 @@
         <v>436</v>
       </c>
       <c r="J68" s="53" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="K68" s="127" t="s">
         <v>340</v>
@@ -8453,7 +8017,7 @@
         <v>379</v>
       </c>
       <c r="M68" s="127" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
     </row>
     <row r="69" spans="1:13" s="128" customFormat="1" ht="75" x14ac:dyDescent="0.25">
@@ -8479,7 +8043,7 @@
         <v>411</v>
       </c>
       <c r="J69" s="130" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="K69" s="130" t="s">
         <v>340</v>
@@ -8488,7 +8052,7 @@
         <v>379</v>
       </c>
       <c r="M69" s="128" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
     </row>
     <row r="70" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -8523,7 +8087,7 @@
         <v>379</v>
       </c>
       <c r="M70" s="127" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
     </row>
     <row r="71" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -8561,7 +8125,7 @@
         <v>379</v>
       </c>
       <c r="M71" s="127" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
     </row>
     <row r="72" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -8596,7 +8160,7 @@
         <v>379</v>
       </c>
       <c r="M72" s="127" t="s">
-        <v>703</v>
+        <v>700</v>
       </c>
     </row>
     <row r="73" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -8631,7 +8195,7 @@
         <v>379</v>
       </c>
       <c r="M73" s="127" t="s">
-        <v>702</v>
+        <v>699</v>
       </c>
     </row>
     <row r="74" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -8669,7 +8233,7 @@
         <v>379</v>
       </c>
       <c r="M74" s="127" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
     </row>
     <row r="75" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -8707,7 +8271,7 @@
         <v>379</v>
       </c>
       <c r="M75" s="127" t="s">
-        <v>700</v>
+        <v>697</v>
       </c>
     </row>
     <row r="76" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -8742,7 +8306,7 @@
         <v>379</v>
       </c>
       <c r="M76" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
     </row>
     <row r="77" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -8780,7 +8344,7 @@
         <v>379</v>
       </c>
       <c r="M77" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
     </row>
     <row r="78" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -8818,7 +8382,7 @@
         <v>379</v>
       </c>
       <c r="M78" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
     </row>
     <row r="79" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -8853,7 +8417,7 @@
         <v>379</v>
       </c>
       <c r="M79" t="s">
-        <v>696</v>
+        <v>693</v>
       </c>
     </row>
     <row r="80" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -8891,7 +8455,7 @@
         <v>379</v>
       </c>
       <c r="M80" s="127" t="s">
-        <v>695</v>
+        <v>692</v>
       </c>
     </row>
     <row r="81" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -8926,7 +8490,7 @@
         <v>379</v>
       </c>
       <c r="M81" s="127" t="s">
-        <v>694</v>
+        <v>691</v>
       </c>
     </row>
     <row r="82" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -8961,7 +8525,7 @@
         <v>379</v>
       </c>
       <c r="M82" s="127" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
     </row>
     <row r="83" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -8996,7 +8560,7 @@
         <v>379</v>
       </c>
       <c r="M83" s="127" t="s">
-        <v>691</v>
+        <v>770</v>
       </c>
     </row>
     <row r="84" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -9031,7 +8595,7 @@
         <v>379</v>
       </c>
       <c r="M84" s="127" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
     </row>
     <row r="85" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -9066,7 +8630,7 @@
         <v>379</v>
       </c>
       <c r="M85" s="127" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
     </row>
     <row r="86" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -9101,7 +8665,7 @@
         <v>379</v>
       </c>
       <c r="M86" s="127" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="87" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -9136,7 +8700,7 @@
         <v>379</v>
       </c>
       <c r="M87" s="127" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="88" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -9171,7 +8735,7 @@
         <v>379</v>
       </c>
       <c r="M88" s="127" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="89" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -9206,7 +8770,7 @@
         <v>379</v>
       </c>
       <c r="M89" s="127" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="90" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -9241,7 +8805,7 @@
         <v>379</v>
       </c>
       <c r="M90" s="127" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="91" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -9276,7 +8840,7 @@
         <v>379</v>
       </c>
       <c r="M91" s="127" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="92" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -9314,7 +8878,7 @@
         <v>379</v>
       </c>
       <c r="M92" s="127" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
     </row>
     <row r="93" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -9349,7 +8913,7 @@
         <v>379</v>
       </c>
       <c r="M93" s="127" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
     </row>
     <row r="94" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -9387,7 +8951,7 @@
         <v>379</v>
       </c>
       <c r="M94" s="127" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="95" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -9422,7 +8986,7 @@
         <v>379</v>
       </c>
       <c r="M95" s="127" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
     </row>
     <row r="96" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -9457,7 +9021,7 @@
         <v>379</v>
       </c>
       <c r="M96" s="127" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
     </row>
     <row r="97" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -9492,7 +9056,7 @@
         <v>379</v>
       </c>
       <c r="M97" s="127" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="98" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -9527,7 +9091,7 @@
         <v>379</v>
       </c>
       <c r="M98" s="127" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
     </row>
     <row r="99" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -9565,7 +9129,7 @@
         <v>379</v>
       </c>
       <c r="M99" s="127" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
     </row>
     <row r="100" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -9600,7 +9164,7 @@
         <v>379</v>
       </c>
       <c r="M100" s="127" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
     </row>
     <row r="101" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -9638,7 +9202,7 @@
         <v>379</v>
       </c>
       <c r="M101" s="127" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
     </row>
     <row r="102" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -9673,7 +9237,7 @@
         <v>379</v>
       </c>
       <c r="M102" s="127" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
     </row>
     <row r="103" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -9708,7 +9272,7 @@
         <v>379</v>
       </c>
       <c r="M103" s="127" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
     </row>
     <row r="104" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -9746,7 +9310,7 @@
         <v>379</v>
       </c>
       <c r="M104" s="127" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
     </row>
     <row r="105" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -9784,7 +9348,7 @@
         <v>379</v>
       </c>
       <c r="M105" s="127" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
     </row>
     <row r="106" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -9819,7 +9383,7 @@
         <v>379</v>
       </c>
       <c r="M106" s="127" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="107" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -9857,7 +9421,7 @@
         <v>379</v>
       </c>
       <c r="M107" s="127" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
     </row>
     <row r="108" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -9892,7 +9456,7 @@
         <v>379</v>
       </c>
       <c r="M108" s="127" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="109" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -9912,7 +9476,7 @@
         <v>39</v>
       </c>
       <c r="G109" s="2" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="I109" t="s">
         <v>411</v>
@@ -9927,7 +9491,7 @@
         <v>379</v>
       </c>
       <c r="M109" s="127" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
     </row>
     <row r="110" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -9962,7 +9526,7 @@
         <v>379</v>
       </c>
       <c r="M110" s="127" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="111" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -9997,7 +9561,7 @@
         <v>379</v>
       </c>
       <c r="M111" s="127" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="112" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -10035,7 +9599,7 @@
         <v>379</v>
       </c>
       <c r="M112" s="127" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="113" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -10073,7 +9637,7 @@
         <v>379</v>
       </c>
       <c r="M113" s="127" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="114" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -10111,7 +9675,7 @@
         <v>379</v>
       </c>
       <c r="M114" s="127" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
     </row>
     <row r="115" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -10146,7 +9710,7 @@
         <v>379</v>
       </c>
       <c r="M115" s="127" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
     </row>
     <row r="116" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -10184,7 +9748,7 @@
         <v>379</v>
       </c>
       <c r="M116" s="127" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
     </row>
     <row r="117" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -10219,7 +9783,7 @@
         <v>379</v>
       </c>
       <c r="M117" s="127" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
     </row>
     <row r="118" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -10254,7 +9818,7 @@
         <v>379</v>
       </c>
       <c r="M118" s="127" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
     </row>
     <row r="119" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -10289,7 +9853,7 @@
         <v>379</v>
       </c>
       <c r="M119" s="127" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="120" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -10324,7 +9888,7 @@
         <v>379</v>
       </c>
       <c r="M120" s="127" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="121" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -10359,7 +9923,7 @@
         <v>379</v>
       </c>
       <c r="M121" s="127" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="122" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -10394,7 +9958,7 @@
         <v>379</v>
       </c>
       <c r="M122" s="127" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="123" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -10429,7 +9993,7 @@
         <v>379</v>
       </c>
       <c r="M123" s="127" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
     </row>
     <row r="124" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -10464,7 +10028,7 @@
         <v>379</v>
       </c>
       <c r="M124" s="127" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="125" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -10499,7 +10063,7 @@
         <v>379</v>
       </c>
       <c r="M125" s="127" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="126" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -10534,7 +10098,7 @@
         <v>379</v>
       </c>
       <c r="M126" s="127" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="127" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -10569,7 +10133,7 @@
         <v>379</v>
       </c>
       <c r="M127" s="127" t="s">
-        <v>646</v>
+        <v>771</v>
       </c>
     </row>
     <row r="128" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -10604,7 +10168,7 @@
         <v>379</v>
       </c>
       <c r="M128" s="127" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="129" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -10639,7 +10203,7 @@
         <v>379</v>
       </c>
       <c r="M129" s="127" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="130" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -10674,7 +10238,7 @@
         <v>379</v>
       </c>
       <c r="M130" s="127" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="131" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -10709,7 +10273,7 @@
         <v>379</v>
       </c>
       <c r="M131" s="127" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="132" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -10744,7 +10308,7 @@
         <v>379</v>
       </c>
       <c r="M132" s="127" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="133" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -10779,7 +10343,7 @@
         <v>379</v>
       </c>
       <c r="M133" s="127" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="134" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -10814,7 +10378,7 @@
         <v>379</v>
       </c>
       <c r="M134" s="127" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="135" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -10849,7 +10413,7 @@
         <v>379</v>
       </c>
       <c r="M135" s="127" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="136" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -10884,7 +10448,7 @@
         <v>379</v>
       </c>
       <c r="M136" s="127" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="137" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -10919,7 +10483,7 @@
         <v>379</v>
       </c>
       <c r="M137" s="127" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="138" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -10954,7 +10518,7 @@
         <v>379</v>
       </c>
       <c r="M138" s="127" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="139" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -10989,7 +10553,7 @@
         <v>379</v>
       </c>
       <c r="M139" s="127" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="140" spans="1:13" ht="60" x14ac:dyDescent="0.25">
@@ -11024,7 +10588,7 @@
         <v>379</v>
       </c>
       <c r="M140" s="127" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="141" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -11062,7 +10626,7 @@
         <v>379</v>
       </c>
       <c r="M141" s="127" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="142" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -11097,7 +10661,7 @@
         <v>379</v>
       </c>
       <c r="M142" s="127" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="143" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -11135,7 +10699,7 @@
         <v>379</v>
       </c>
       <c r="M143" s="127" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="144" spans="1:13" ht="90" x14ac:dyDescent="0.25">
@@ -11170,7 +10734,7 @@
         <v>379</v>
       </c>
       <c r="M144" s="127" t="s">
-        <v>629</v>
+        <v>772</v>
       </c>
     </row>
     <row r="145" spans="1:13" ht="75" x14ac:dyDescent="0.25">
@@ -11358,15 +10922,15 @@
     <sortCondition ref="D2:D149"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{E9AA0514-4F1F-4D48-9ADD-4471FD4B0607}">
-      <pane ySplit="1" topLeftCell="A145" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
+    <customSheetView guid="{0B508B25-7123-447E-9FD5-FE20BBAD71B2}" scale="70">
+      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G141" sqref="G141"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
     </customSheetView>
-    <customSheetView guid="{D89975A1-9A50-491E-B44B-6A9DDF60C5E2}" topLeftCell="F1">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K158" sqref="K158"/>
+    <customSheetView guid="{EDE4CE66-77B3-4DE9-B8E1-41F2D0C67E38}">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
     </customSheetView>
@@ -11376,15 +10940,15 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
     </customSheetView>
-    <customSheetView guid="{EDE4CE66-77B3-4DE9-B8E1-41F2D0C67E38}">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G25" sqref="G25"/>
+    <customSheetView guid="{D89975A1-9A50-491E-B44B-6A9DDF60C5E2}" topLeftCell="F1">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K158" sqref="K158"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
     </customSheetView>
-    <customSheetView guid="{0B508B25-7123-447E-9FD5-FE20BBAD71B2}" scale="70">
-      <pane ySplit="1" topLeftCell="A135" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G141" sqref="G141"/>
+    <customSheetView guid="{E9AA0514-4F1F-4D48-9ADD-4471FD4B0607}">
+      <pane ySplit="1" topLeftCell="A145" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
     </customSheetView>
@@ -11398,8 +10962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection sqref="A1:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11667,24 +11231,24 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E9AA0514-4F1F-4D48-9ADD-4471FD4B0607}">
+    <customSheetView guid="{0B508B25-7123-447E-9FD5-FE20BBAD71B2}" topLeftCell="A10">
+      <selection activeCell="D11" sqref="D11"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{EDE4CE66-77B3-4DE9-B8E1-41F2D0C67E38}">
       <selection activeCell="C6" sqref="C6"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{22AF5D13-DA6D-4567-8DD6-5735431A3EE3}" topLeftCell="A4">
+      <selection activeCell="D14" sqref="D14"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
     </customSheetView>
     <customSheetView guid="{D89975A1-9A50-491E-B44B-6A9DDF60C5E2}">
       <selection activeCell="C15" sqref="C15"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{22AF5D13-DA6D-4567-8DD6-5735431A3EE3}" topLeftCell="A4">
-      <selection activeCell="D14" sqref="D14"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{EDE4CE66-77B3-4DE9-B8E1-41F2D0C67E38}">
+    <customSheetView guid="{E9AA0514-4F1F-4D48-9ADD-4471FD4B0607}">
       <selection activeCell="C6" sqref="C6"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{0B508B25-7123-447E-9FD5-FE20BBAD71B2}" topLeftCell="A10">
-      <selection activeCell="D11" sqref="D11"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -11839,7 +11403,15 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E9AA0514-4F1F-4D48-9ADD-4471FD4B0607}">
+    <customSheetView guid="{0B508B25-7123-447E-9FD5-FE20BBAD71B2}">
+      <selection activeCell="D9" sqref="D9"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{EDE4CE66-77B3-4DE9-B8E1-41F2D0C67E38}">
+      <selection activeCell="D9" sqref="D9"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{22AF5D13-DA6D-4567-8DD6-5735431A3EE3}">
       <selection activeCell="D9" sqref="D9"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -11847,15 +11419,7 @@
       <selection activeCell="F1" sqref="F1:F1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{22AF5D13-DA6D-4567-8DD6-5735431A3EE3}">
-      <selection activeCell="D9" sqref="D9"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{EDE4CE66-77B3-4DE9-B8E1-41F2D0C67E38}">
-      <selection activeCell="D9" sqref="D9"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{0B508B25-7123-447E-9FD5-FE20BBAD71B2}">
+    <customSheetView guid="{E9AA0514-4F1F-4D48-9ADD-4471FD4B0607}">
       <selection activeCell="D9" sqref="D9"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -11960,7 +11524,15 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{E9AA0514-4F1F-4D48-9ADD-4471FD4B0607}">
+    <customSheetView guid="{0B508B25-7123-447E-9FD5-FE20BBAD71B2}">
+      <selection activeCell="D6" sqref="D6"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{EDE4CE66-77B3-4DE9-B8E1-41F2D0C67E38}">
+      <selection activeCell="D6" sqref="D6"/>
+      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+    </customSheetView>
+    <customSheetView guid="{22AF5D13-DA6D-4567-8DD6-5735431A3EE3}">
       <selection activeCell="D6" sqref="D6"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -11968,15 +11540,7 @@
       <selection activeCell="F1" sqref="F1:F1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{22AF5D13-DA6D-4567-8DD6-5735431A3EE3}">
-      <selection activeCell="D6" sqref="D6"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{EDE4CE66-77B3-4DE9-B8E1-41F2D0C67E38}">
-      <selection activeCell="D6" sqref="D6"/>
-      <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{0B508B25-7123-447E-9FD5-FE20BBAD71B2}">
+    <customSheetView guid="{E9AA0514-4F1F-4D48-9ADD-4471FD4B0607}">
       <selection activeCell="D6" sqref="D6"/>
       <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
     </customSheetView>

</xml_diff>